<commit_message>
Membuat keputusan_tindakan menjadi array
</commit_message>
<xml_diff>
--- a/public/template/template_data_siswa.xlsx
+++ b/public/template/template_data_siswa.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mario Klau\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projek Web\web-tatib\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5D5214-3A44-4DCA-A4A5-6AAC56AAA988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA5E05A-9A0C-4A63-B5F4-99E31AE7AEB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FECFA93F-536F-4547-9EA8-F1846CDB17C0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Nama Siswa</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Kode_Kelas</t>
+  </si>
+  <si>
+    <t>NIS</t>
   </si>
 </sst>
 </file>
@@ -128,8 +131,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Sel Periksa" xfId="1" builtinId="23"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -145,7 +148,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -441,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F039FAC-40C6-4A1B-A777-C3CA0941360D}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -452,10 +455,11 @@
     <col min="1" max="1" width="15.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="35" style="1" customWidth="1"/>
     <col min="3" max="3" width="21.6640625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="22.109375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -463,10 +467,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:4" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>